<commit_message>
Checking in latest updates for NASONLINE Scripts
Checking in Updated Excel Spreadsheets
</commit_message>
<xml_diff>
--- a/utilities/Excel_Sheets/Products/ADULTDC.xlsx
+++ b/utilities/Excel_Sheets/Products/ADULTDC.xlsx
@@ -473,7 +473,7 @@
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -540,7 +540,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>43332</v>
+        <v>43377</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
@@ -580,7 +580,7 @@
       </c>
       <c r="C4" s="6">
         <f ca="1">TODAY()</f>
-        <v>43332</v>
+        <v>43377</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>3</v>
@@ -620,7 +620,7 @@
       </c>
       <c r="C6" s="6">
         <f ca="1">TODAY()</f>
-        <v>43332</v>
+        <v>43377</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>3</v>
@@ -673,7 +673,7 @@
       </c>
       <c r="C8" s="6">
         <f ca="1">TODAY()</f>
-        <v>43332</v>
+        <v>43377</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>3</v>
@@ -726,7 +726,7 @@
       </c>
       <c r="C10" s="6">
         <f ca="1">TODAY()</f>
-        <v>43332</v>
+        <v>43377</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>3</v>
@@ -779,7 +779,7 @@
       </c>
       <c r="C12" s="6">
         <f ca="1">TODAY()</f>
-        <v>43332</v>
+        <v>43377</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>3</v>
@@ -832,7 +832,7 @@
       </c>
       <c r="C14" s="6">
         <f ca="1">TODAY()</f>
-        <v>43332</v>
+        <v>43377</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>3</v>
@@ -885,7 +885,7 @@
       </c>
       <c r="C16" s="6">
         <f ca="1">TODAY()</f>
-        <v>43332</v>
+        <v>43377</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>3</v>

</xml_diff>